<commit_message>
Memcached db - run + workload A
- add new DB called Memcached
- run db
- testing workload A + saving output data
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4BA881-5900-432A-8BF1-441E150DCE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F2C299-996E-4A96-AFB9-AEEE0AB0B78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workloads - data" sheetId="1" r:id="rId1"/>
     <sheet name="Redis" sheetId="2" r:id="rId2"/>
     <sheet name="Riak" sheetId="3" r:id="rId3"/>
     <sheet name="Aerospike" sheetId="4" r:id="rId4"/>
+    <sheet name="Memcached" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="21">
   <si>
     <t>DB</t>
   </si>
@@ -99,6 +100,9 @@
   </si>
   <si>
     <t>50 272</t>
+  </si>
+  <si>
+    <t>Memcached</t>
   </si>
 </sst>
 </file>
@@ -230,9 +234,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - data'!$C$3:$E$3</c:f>
+              <c:f>'Workloads - data'!$C$3:$F$3</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
@@ -242,15 +246,18 @@
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>Memcached</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$16:$E$16</c:f>
+              <c:f>'Workloads - data'!$C$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1264.6666666666667</c:v>
                 </c:pt>
@@ -259,6 +266,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1121</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1363</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,9 +528,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - data'!$C$3:$E$3</c:f>
+              <c:f>'Workloads - data'!$C$3:$F$3</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
@@ -530,15 +540,18 @@
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>Memcached</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$17:$E$17</c:f>
+              <c:f>'Workloads - data'!$C$17:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1891.6666666666667</c:v>
                 </c:pt>
@@ -547,6 +560,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1538.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1758</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8240,10 +8256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8252,12 +8268,12 @@
     <col min="4" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -8270,8 +8286,11 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -8287,8 +8306,12 @@
         <f>Aerospike!C8</f>
         <v>196849.33333333334</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f>Memcached!D8</f>
+        <v>241009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -8304,8 +8327,12 @@
         <f>Aerospike!C9</f>
         <v>5081.1244477222363</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f>Memcached!D9</f>
+        <v>4149.2226431378003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -8324,8 +8351,12 @@
         <f>Aerospike!C10</f>
         <v>499106</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f>Memcached!D10</f>
+        <v>500683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -8341,8 +8372,12 @@
         <f>Aerospike!C11</f>
         <v>785.8631093017184</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f>Memcached!D11</f>
+        <v>958.95825702090895</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -8358,8 +8393,12 @@
         <f>Aerospike!C12</f>
         <v>319.66666666666669</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f>Memcached!D12</f>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -8375,8 +8414,12 @@
         <f>Aerospike!C13</f>
         <v>27311</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f>Memcached!D13</f>
+        <v>80511</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -8392,8 +8435,12 @@
         <f>Aerospike!C14</f>
         <v>1122.6666666666667</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>Memcached!D14</f>
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -8409,8 +8456,12 @@
         <f>Aerospike!C15</f>
         <v>1540.3333333333333</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f>Memcached!D15</f>
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -8429,8 +8480,12 @@
         <f>Aerospike!C16</f>
         <v>500894</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f>Memcached!D16</f>
+        <v>499317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -8446,8 +8501,12 @@
         <f>Aerospike!C17</f>
         <v>782.67998551661094</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f>Memcached!D17</f>
+        <v>958.12489460603103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -8463,8 +8522,12 @@
         <f>Aerospike!C18</f>
         <v>314.33333333333331</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f>Memcached!D18</f>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -8480,8 +8543,12 @@
         <f>Aerospike!C19</f>
         <v>29753.666666666668</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f>Memcached!D19</f>
+        <v>64031</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -8497,8 +8564,12 @@
         <f>Aerospike!C20</f>
         <v>1121</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f>Memcached!D20</f>
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -8514,13 +8585,17 @@
         <f>Aerospike!C21</f>
         <v>1538.3333333333333</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f>Memcached!D21</f>
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -8533,8 +8608,11 @@
       <c r="E22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -8551,7 +8629,7 @@
         <v>202264</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>5</v>
       </c>
@@ -8568,7 +8646,7 @@
         <v>4945.3776482559506</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -8588,7 +8666,7 @@
         <v>949706</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>8</v>
       </c>
@@ -8605,7 +8683,7 @@
         <v>805.96629449109275</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -8622,7 +8700,7 @@
         <v>313.33333333333331</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -8639,7 +8717,7 @@
         <v>25732.333333333332</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -8656,7 +8734,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>13</v>
       </c>
@@ -8673,7 +8751,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -8693,7 +8771,7 @@
         <v>50294</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>8</v>
       </c>
@@ -8710,7 +8788,7 @@
         <v>809.97773750073532</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>10</v>
       </c>
@@ -8727,7 +8805,7 @@
         <v>341.33333333333331</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -8744,7 +8822,7 @@
         <v>17132.333333333332</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>12</v>
       </c>
@@ -8761,7 +8839,7 @@
         <v>1197.6666666666667</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>13</v>
       </c>
@@ -8778,12 +8856,12 @@
         <v>1779.6666666666667</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -8796,8 +8874,11 @@
       <c r="E41" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>4</v>
       </c>
@@ -8814,7 +8895,7 @@
         <v>209528</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>5</v>
       </c>
@@ -8831,7 +8912,7 @@
         <v>4778.1274961757899</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -8851,7 +8932,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>8</v>
       </c>
@@ -8868,7 +8949,7 @@
         <v>835.167418</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>10</v>
       </c>
@@ -8885,7 +8966,7 @@
         <v>319.33333333333331</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>11</v>
       </c>
@@ -8902,7 +8983,7 @@
         <v>41881.666666666664</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>12</v>
       </c>
@@ -8946,8 +9027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA6185-A47A-430A-AEC2-7ED0A4C5D4C7}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10984,4 +11065,558 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C80EE16-73D0-4778-A1BC-D419AAA6A283}">
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGEA(D8:F8)</f>
+        <v>243409.33333333334</v>
+      </c>
+      <c r="D8">
+        <v>241009</v>
+      </c>
+      <c r="E8">
+        <v>242527</v>
+      </c>
+      <c r="F8">
+        <v>246692</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:C21" si="0">AVERAGEA(D9:F9)</f>
+        <v>4108.7042113635098</v>
+      </c>
+      <c r="D9">
+        <v>4149.2226431378003</v>
+      </c>
+      <c r="E9">
+        <v>4123.2522564497904</v>
+      </c>
+      <c r="F9">
+        <v>4053.63773450294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <f>D10</f>
+        <v>500683</v>
+      </c>
+      <c r="D10">
+        <v>500683</v>
+      </c>
+      <c r="E10">
+        <v>501166</v>
+      </c>
+      <c r="F10">
+        <v>499564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>967.90216610373329</v>
+      </c>
+      <c r="D11">
+        <v>958.95825702090895</v>
+      </c>
+      <c r="E11">
+        <v>963.71946820015705</v>
+      </c>
+      <c r="F11">
+        <v>981.028773090134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>395.33333333333331</v>
+      </c>
+      <c r="D12">
+        <v>391</v>
+      </c>
+      <c r="E12">
+        <v>395</v>
+      </c>
+      <c r="F12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>83177.666666666672</v>
+      </c>
+      <c r="D13">
+        <v>80511</v>
+      </c>
+      <c r="E13">
+        <v>67519</v>
+      </c>
+      <c r="F13">
+        <v>101503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1385</v>
+      </c>
+      <c r="D14">
+        <v>1362</v>
+      </c>
+      <c r="E14">
+        <v>1370</v>
+      </c>
+      <c r="F14">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1846</v>
+      </c>
+      <c r="D15">
+        <v>1767</v>
+      </c>
+      <c r="E15">
+        <v>1788</v>
+      </c>
+      <c r="F15">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <f>D16</f>
+        <v>499317</v>
+      </c>
+      <c r="D16">
+        <v>499317</v>
+      </c>
+      <c r="E16">
+        <v>498834</v>
+      </c>
+      <c r="F16">
+        <v>500436</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>967.90354078356597</v>
+      </c>
+      <c r="D17">
+        <v>958.12489460603103</v>
+      </c>
+      <c r="E17">
+        <v>964.71301475039797</v>
+      </c>
+      <c r="F17">
+        <v>980.87271299426902</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>407.66666666666669</v>
+      </c>
+      <c r="D18">
+        <v>415</v>
+      </c>
+      <c r="E18">
+        <v>403</v>
+      </c>
+      <c r="F18">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>82249.666666666672</v>
+      </c>
+      <c r="D19">
+        <v>64031</v>
+      </c>
+      <c r="E19">
+        <v>81663</v>
+      </c>
+      <c r="F19">
+        <v>101055</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1387.6666666666667</v>
+      </c>
+      <c r="D20">
+        <v>1363</v>
+      </c>
+      <c r="E20">
+        <v>1374</v>
+      </c>
+      <c r="F20">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>1850.6666666666667</v>
+      </c>
+      <c r="D21">
+        <v>1758</v>
+      </c>
+      <c r="E21">
+        <v>1789</v>
+      </c>
+      <c r="F21">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="e">
+        <f>AVERAGEA(D27:F27)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="e">
+        <f t="shared" ref="C28:C40" si="1">AVERAGEA(D28:F28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29">
+        <f>D29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <f>D35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" t="e">
+        <f>AVERAGEA(D46:F46)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="e">
+        <f t="shared" ref="C47:C53" si="2">AVERAGEA(D47:F47)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48">
+        <f>D48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="e">
+        <f>AVERAGEA(D49:F49)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Memcached - Workload C test 1,2,3
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F2C299-996E-4A96-AFB9-AEEE0AB0B78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F6760F-A32D-45C6-A47A-0038E83A2740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workloads - data" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,7 @@
                   <c:v>1121</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1363</c:v>
+                  <c:v>1387.6666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -562,7 +562,7 @@
                   <c:v>1538.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1758</c:v>
+                  <c:v>1850.6666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8258,8 +8258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8307,8 +8307,8 @@
         <v>196849.33333333334</v>
       </c>
       <c r="F4">
-        <f>Memcached!D8</f>
-        <v>241009</v>
+        <f>Memcached!C8</f>
+        <v>243409.33333333334</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -8328,8 +8328,8 @@
         <v>5081.1244477222363</v>
       </c>
       <c r="F5">
-        <f>Memcached!D9</f>
-        <v>4149.2226431378003</v>
+        <f>Memcached!C9</f>
+        <v>4108.7042113635098</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -8352,7 +8352,7 @@
         <v>499106</v>
       </c>
       <c r="F6">
-        <f>Memcached!D10</f>
+        <f>Memcached!C10</f>
         <v>500683</v>
       </c>
     </row>
@@ -8373,8 +8373,8 @@
         <v>785.8631093017184</v>
       </c>
       <c r="F7">
-        <f>Memcached!D11</f>
-        <v>958.95825702090895</v>
+        <f>Memcached!C11</f>
+        <v>967.90216610373329</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -8394,8 +8394,8 @@
         <v>319.66666666666669</v>
       </c>
       <c r="F8">
-        <f>Memcached!D12</f>
-        <v>391</v>
+        <f>Memcached!C12</f>
+        <v>395.33333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -8415,8 +8415,8 @@
         <v>27311</v>
       </c>
       <c r="F9">
-        <f>Memcached!D13</f>
-        <v>80511</v>
+        <f>Memcached!C13</f>
+        <v>83177.666666666672</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -8436,8 +8436,8 @@
         <v>1122.6666666666667</v>
       </c>
       <c r="F10">
-        <f>Memcached!D14</f>
-        <v>1362</v>
+        <f>Memcached!C14</f>
+        <v>1385</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -8457,8 +8457,8 @@
         <v>1540.3333333333333</v>
       </c>
       <c r="F11">
-        <f>Memcached!D15</f>
-        <v>1767</v>
+        <f>Memcached!C15</f>
+        <v>1846</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -8481,7 +8481,7 @@
         <v>500894</v>
       </c>
       <c r="F12">
-        <f>Memcached!D16</f>
+        <f>Memcached!C16</f>
         <v>499317</v>
       </c>
     </row>
@@ -8502,8 +8502,8 @@
         <v>782.67998551661094</v>
       </c>
       <c r="F13">
-        <f>Memcached!D17</f>
-        <v>958.12489460603103</v>
+        <f>Memcached!C17</f>
+        <v>967.90354078356597</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -8523,8 +8523,8 @@
         <v>314.33333333333331</v>
       </c>
       <c r="F14">
-        <f>Memcached!D18</f>
-        <v>415</v>
+        <f>Memcached!C18</f>
+        <v>407.66666666666669</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -8544,8 +8544,8 @@
         <v>29753.666666666668</v>
       </c>
       <c r="F15">
-        <f>Memcached!D19</f>
-        <v>64031</v>
+        <f>Memcached!C19</f>
+        <v>82249.666666666672</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -8565,8 +8565,8 @@
         <v>1121</v>
       </c>
       <c r="F16">
-        <f>Memcached!D20</f>
-        <v>1363</v>
+        <f>Memcached!C20</f>
+        <v>1387.6666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -8586,8 +8586,8 @@
         <v>1538.3333333333333</v>
       </c>
       <c r="F17">
-        <f>Memcached!D21</f>
-        <v>1758</v>
+        <f>Memcached!C21</f>
+        <v>1850.6666666666667</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -8628,6 +8628,10 @@
         <f>Aerospike!C27</f>
         <v>202264</v>
       </c>
+      <c r="F23" t="e">
+        <f>Memcached!C27</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -8645,6 +8649,10 @@
         <f>Aerospike!C28</f>
         <v>4945.3776482559506</v>
       </c>
+      <c r="F24" t="e">
+        <f>Memcached!C28</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -8665,6 +8673,10 @@
         <f>Aerospike!C29</f>
         <v>949706</v>
       </c>
+      <c r="F25">
+        <f>Memcached!C29</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -8682,6 +8694,10 @@
         <f>Aerospike!C30</f>
         <v>805.96629449109275</v>
       </c>
+      <c r="F26" t="e">
+        <f>Memcached!C30</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -8699,6 +8715,10 @@
         <f>Aerospike!C31</f>
         <v>313.33333333333331</v>
       </c>
+      <c r="F27" t="e">
+        <f>Memcached!C31</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -8716,6 +8736,10 @@
         <f>Aerospike!C32</f>
         <v>25732.333333333332</v>
       </c>
+      <c r="F28" t="e">
+        <f>Memcached!C32</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -8733,6 +8757,10 @@
         <f>Aerospike!C33</f>
         <v>1188</v>
       </c>
+      <c r="F29" t="e">
+        <f>Memcached!C33</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -8750,6 +8778,10 @@
         <f>Aerospike!C34</f>
         <v>1756</v>
       </c>
+      <c r="F30" t="e">
+        <f>Memcached!C34</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -8770,6 +8802,10 @@
         <f>Aerospike!C35</f>
         <v>50294</v>
       </c>
+      <c r="F31">
+        <f>Memcached!C35</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -8787,6 +8823,10 @@
         <f>Aerospike!C36</f>
         <v>809.97773750073532</v>
       </c>
+      <c r="F32" t="e">
+        <f>Memcached!C36</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
@@ -8804,6 +8844,10 @@
         <f>Aerospike!C37</f>
         <v>341.33333333333331</v>
       </c>
+      <c r="F33" t="e">
+        <f>Memcached!C37</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
@@ -8821,6 +8865,10 @@
         <f>Aerospike!C38</f>
         <v>17132.333333333332</v>
       </c>
+      <c r="F34" t="e">
+        <f>Memcached!C38</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -8838,6 +8886,10 @@
         <f>Aerospike!C39</f>
         <v>1197.6666666666667</v>
       </c>
+      <c r="F35" t="e">
+        <f>Memcached!C39</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -8855,6 +8907,10 @@
         <f>Aerospike!C40</f>
         <v>1779.6666666666667</v>
       </c>
+      <c r="F36" t="e">
+        <f>Memcached!C40</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -8894,6 +8950,10 @@
         <f>Aerospike!C46</f>
         <v>209528</v>
       </c>
+      <c r="F42">
+        <f>Memcached!C46</f>
+        <v>221353.33333333334</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
@@ -8911,6 +8971,10 @@
         <f>Aerospike!C47</f>
         <v>4778.1274961757899</v>
       </c>
+      <c r="F43">
+        <f>Memcached!C47</f>
+        <v>4517.6713328397063</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -8931,6 +8995,10 @@
         <f>Aerospike!C48</f>
         <v>1000000</v>
       </c>
+      <c r="F44">
+        <f>Memcached!C48</f>
+        <v>1000000</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -8948,6 +9016,10 @@
         <f>Aerospike!C49</f>
         <v>835.167418</v>
       </c>
+      <c r="F45">
+        <f>Memcached!C49</f>
+        <v>880.1736556666666</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -8965,6 +9037,10 @@
         <f>Aerospike!C50</f>
         <v>319.33333333333331</v>
       </c>
+      <c r="F46">
+        <f>Memcached!C50</f>
+        <v>376</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
@@ -8982,6 +9058,10 @@
         <f>Aerospike!C51</f>
         <v>41881.666666666664</v>
       </c>
+      <c r="F47">
+        <f>Memcached!C51</f>
+        <v>39071</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
@@ -8999,8 +9079,12 @@
         <f>Aerospike!C52</f>
         <v>1242.3333333333333</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f>Memcached!C52</f>
+        <v>1233.3333333333333</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>13</v>
       </c>
@@ -9015,6 +9099,10 @@
       <c r="E49">
         <f>Aerospike!C53</f>
         <v>1861.6666666666667</v>
+      </c>
+      <c r="F49">
+        <f>Memcached!C53</f>
+        <v>1615.3333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -9027,8 +9115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA6185-A47A-430A-AEC2-7ED0A4C5D4C7}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11071,8 +11159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C80EE16-73D0-4778-A1BC-D419AAA6A283}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11545,18 +11633,36 @@
       <c r="B46" t="s">
         <v>4</v>
       </c>
-      <c r="C46" t="e">
+      <c r="C46">
         <f>AVERAGEA(D46:F46)</f>
-        <v>#DIV/0!</v>
+        <v>221353.33333333334</v>
+      </c>
+      <c r="D46">
+        <v>221716</v>
+      </c>
+      <c r="E46">
+        <v>221312</v>
+      </c>
+      <c r="F46">
+        <v>221032</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>5</v>
       </c>
-      <c r="C47" t="e">
+      <c r="C47">
         <f t="shared" ref="C47:C53" si="2">AVERAGEA(D47:F47)</f>
-        <v>#DIV/0!</v>
+        <v>4517.6713328397063</v>
+      </c>
+      <c r="D47">
+        <v>4510.2744050948004</v>
+      </c>
+      <c r="E47">
+        <v>4518.5078079814903</v>
+      </c>
+      <c r="F47">
+        <v>4524.2317854428302</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -11568,52 +11674,106 @@
       </c>
       <c r="C48">
         <f>D48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1000000</v>
+      </c>
+      <c r="D48">
+        <v>1000000</v>
+      </c>
+      <c r="E48">
+        <v>1000000</v>
+      </c>
+      <c r="F48">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>8</v>
       </c>
-      <c r="C49" t="e">
+      <c r="C49">
         <f>AVERAGEA(D49:F49)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+        <v>880.1736556666666</v>
+      </c>
+      <c r="D49">
+        <v>881.60456099999999</v>
+      </c>
+      <c r="E49">
+        <v>880.207448</v>
+      </c>
+      <c r="F49">
+        <v>878.70895800000005</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>10</v>
       </c>
-      <c r="C50" t="e">
+      <c r="C50">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+      <c r="D50">
+        <v>385</v>
+      </c>
+      <c r="E50">
+        <v>354</v>
+      </c>
+      <c r="F50">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>11</v>
       </c>
-      <c r="C51" t="e">
+      <c r="C51">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+        <v>39071</v>
+      </c>
+      <c r="D51">
+        <v>65279</v>
+      </c>
+      <c r="E51">
+        <v>22719</v>
+      </c>
+      <c r="F51">
+        <v>29215</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>12</v>
       </c>
-      <c r="C52" t="e">
+      <c r="C52">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1233.3333333333333</v>
+      </c>
+      <c r="D52">
+        <v>1235</v>
+      </c>
+      <c r="E52">
+        <v>1237</v>
+      </c>
+      <c r="F52">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>13</v>
       </c>
-      <c r="C53" t="e">
+      <c r="C53">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1615.3333333333333</v>
+      </c>
+      <c r="D53">
+        <v>1605</v>
+      </c>
+      <c r="E53">
+        <v>1629</v>
+      </c>
+      <c r="F53">
+        <v>1612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finishing Memcached and Riak tests
- Memcached tests B 1,2,3; C 1,2,3
- Riak tests A 2,3; B 2,3; C 2,3
- TMP file for some tests outputs
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F6760F-A32D-45C6-A47A-0038E83A2740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41143081-BC4A-4758-A404-D5E274083C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workloads - data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="20">
   <si>
     <t>DB</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Workload C - Read-only</t>
-  </si>
-  <si>
-    <t>50 272</t>
   </si>
   <si>
     <t>Memcached</t>
@@ -262,7 +259,7 @@
                   <c:v>1264.6666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8951</c:v>
+                  <c:v>9819</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1121</c:v>
@@ -556,7 +553,7 @@
                   <c:v>1891.6666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14215</c:v>
+                  <c:v>16332.333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1538.3333333333333</c:v>
@@ -847,7 +844,7 @@
                   <c:v>1322.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8487</c:v>
+                  <c:v>8903</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1197.6666666666667</c:v>
@@ -1135,7 +1132,7 @@
                   <c:v>2243.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13559</c:v>
+                  <c:v>14495</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1779.6666666666667</c:v>
@@ -1423,7 +1420,7 @@
                   <c:v>1213.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3511</c:v>
+                  <c:v>3714.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1242.3333333333333</c:v>
@@ -1711,7 +1708,7 @@
                   <c:v>1856</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6939</c:v>
+                  <c:v>7885.666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1861.6666666666667</c:v>
@@ -1999,7 +1996,7 @@
                   <c:v>4801.03800056401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1253.75499621366</c:v>
+                  <c:v>1283.9777176479602</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5081.1244477222363</c:v>
@@ -2287,7 +2284,7 @@
                   <c:v>4726.9578685717897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1823.2305092100401</c:v>
+                  <c:v>1778.1582630532967</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4945.3776482559506</c:v>
@@ -2575,7 +2572,7 @@
                   <c:v>4868.3014319549338</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1851.7901255143299</c:v>
+                  <c:v>1783.3907950035066</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4778.1274961757899</c:v>
@@ -8258,8 +8255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8287,7 +8284,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8300,7 +8297,7 @@
       </c>
       <c r="D4">
         <f>Riak!C8</f>
-        <v>797604</v>
+        <v>803880.33333333337</v>
       </c>
       <c r="E4">
         <f>Aerospike!C8</f>
@@ -8321,7 +8318,7 @@
       </c>
       <c r="D5">
         <f>Riak!C9</f>
-        <v>1253.75499621366</v>
+        <v>1283.9777176479602</v>
       </c>
       <c r="E5">
         <f>Aerospike!C9</f>
@@ -8366,7 +8363,7 @@
       </c>
       <c r="D7">
         <f>Riak!C11</f>
-        <v>2054.67928302776</v>
+        <v>2175.8569730388999</v>
       </c>
       <c r="E7">
         <f>Aerospike!C11</f>
@@ -8387,7 +8384,7 @@
       </c>
       <c r="D8">
         <f>Riak!C12</f>
-        <v>858</v>
+        <v>861.33333333333337</v>
       </c>
       <c r="E8">
         <f>Aerospike!C12</f>
@@ -8408,7 +8405,7 @@
       </c>
       <c r="D9">
         <f>Riak!C13</f>
-        <v>169855</v>
+        <v>158271</v>
       </c>
       <c r="E9">
         <f>Aerospike!C13</f>
@@ -8429,7 +8426,7 @@
       </c>
       <c r="D10">
         <f>Riak!C14</f>
-        <v>3311</v>
+        <v>3695</v>
       </c>
       <c r="E10">
         <f>Aerospike!C14</f>
@@ -8450,7 +8447,7 @@
       </c>
       <c r="D11">
         <f>Riak!C15</f>
-        <v>6375</v>
+        <v>7399</v>
       </c>
       <c r="E11">
         <f>Aerospike!C15</f>
@@ -8495,7 +8492,7 @@
       </c>
       <c r="D13">
         <f>Riak!C17</f>
-        <v>5649.6048753783698</v>
+        <v>5941.3298998398968</v>
       </c>
       <c r="E13">
         <f>Aerospike!C17</f>
@@ -8516,7 +8513,7 @@
       </c>
       <c r="D14">
         <f>Riak!C18</f>
-        <v>2528</v>
+        <v>2526.6666666666665</v>
       </c>
       <c r="E14">
         <f>Aerospike!C18</f>
@@ -8537,7 +8534,7 @@
       </c>
       <c r="D15">
         <f>Riak!C19</f>
-        <v>176639</v>
+        <v>167764.33333333334</v>
       </c>
       <c r="E15">
         <f>Aerospike!C19</f>
@@ -8558,7 +8555,7 @@
       </c>
       <c r="D16">
         <f>Riak!C20</f>
-        <v>8951</v>
+        <v>9819</v>
       </c>
       <c r="E16">
         <f>Aerospike!C20</f>
@@ -8579,7 +8576,7 @@
       </c>
       <c r="D17">
         <f>Riak!C21</f>
-        <v>14215</v>
+        <v>16332.333333333334</v>
       </c>
       <c r="E17">
         <f>Aerospike!C21</f>
@@ -8609,7 +8606,7 @@
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -8622,15 +8619,15 @@
       </c>
       <c r="D23">
         <f>Riak!C27</f>
-        <v>548477</v>
+        <v>562799.66666666663</v>
       </c>
       <c r="E23">
         <f>Aerospike!C27</f>
         <v>202264</v>
       </c>
-      <c r="F23" t="e">
+      <c r="F23">
         <f>Memcached!C27</f>
-        <v>#DIV/0!</v>
+        <v>263195.66666666669</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -8643,15 +8640,15 @@
       </c>
       <c r="D24">
         <f>Riak!C28</f>
-        <v>1823.2305092100401</v>
+        <v>1778.1582630532967</v>
       </c>
       <c r="E24">
         <f>Aerospike!C28</f>
         <v>4945.3776482559506</v>
       </c>
-      <c r="F24" t="e">
+      <c r="F24">
         <f>Memcached!C28</f>
-        <v>#DIV/0!</v>
+        <v>3863.5883942419064</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -8675,7 +8672,7 @@
       </c>
       <c r="F25">
         <f>Memcached!C29</f>
-        <v>0</v>
+        <v>950435</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -8688,15 +8685,15 @@
       </c>
       <c r="D26">
         <f>Riak!C30</f>
-        <v>2013.5313047525101</v>
+        <v>2072.9082253935767</v>
       </c>
       <c r="E26">
         <f>Aerospike!C30</f>
         <v>805.96629449109275</v>
       </c>
-      <c r="F26" t="e">
+      <c r="F26">
         <f>Memcached!C30</f>
-        <v>#DIV/0!</v>
+        <v>1046.1802303928137</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -8709,15 +8706,15 @@
       </c>
       <c r="D27">
         <f>Riak!C31</f>
-        <v>852</v>
+        <v>825.33333333333337</v>
       </c>
       <c r="E27">
         <f>Aerospike!C31</f>
         <v>313.33333333333331</v>
       </c>
-      <c r="F27" t="e">
+      <c r="F27">
         <f>Memcached!C31</f>
-        <v>#DIV/0!</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -8730,15 +8727,15 @@
       </c>
       <c r="D28">
         <f>Riak!C32</f>
-        <v>82303</v>
+        <v>110356.33333333333</v>
       </c>
       <c r="E28">
         <f>Aerospike!C32</f>
         <v>25732.333333333332</v>
       </c>
-      <c r="F28" t="e">
+      <c r="F28">
         <f>Memcached!C32</f>
-        <v>#DIV/0!</v>
+        <v>112020.33333333333</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -8751,15 +8748,15 @@
       </c>
       <c r="D29">
         <f>Riak!C33</f>
-        <v>3051</v>
+        <v>3232.3333333333335</v>
       </c>
       <c r="E29">
         <f>Aerospike!C33</f>
         <v>1188</v>
       </c>
-      <c r="F29" t="e">
+      <c r="F29">
         <f>Memcached!C33</f>
-        <v>#DIV/0!</v>
+        <v>1735.3333333333333</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -8772,15 +8769,15 @@
       </c>
       <c r="D30">
         <f>Riak!C34</f>
-        <v>6035</v>
+        <v>6805.666666666667</v>
       </c>
       <c r="E30">
         <f>Aerospike!C34</f>
         <v>1756</v>
       </c>
-      <c r="F30" t="e">
+      <c r="F30">
         <f>Memcached!C34</f>
-        <v>#DIV/0!</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -8794,9 +8791,9 @@
         <f>Redis!C35</f>
         <v>50164</v>
       </c>
-      <c r="D31" t="str">
+      <c r="D31">
         <f>Riak!C35</f>
-        <v>50 272</v>
+        <v>50272</v>
       </c>
       <c r="E31">
         <f>Aerospike!C35</f>
@@ -8804,7 +8801,7 @@
       </c>
       <c r="F31">
         <f>Memcached!C35</f>
-        <v>0</v>
+        <v>49565</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -8817,15 +8814,15 @@
       </c>
       <c r="D32">
         <f>Riak!C36</f>
-        <v>5714.9600163461901</v>
+        <v>5827.5136784126071</v>
       </c>
       <c r="E32">
         <f>Aerospike!C36</f>
         <v>809.97773750073532</v>
       </c>
-      <c r="F32" t="e">
+      <c r="F32">
         <f>Memcached!C36</f>
-        <v>#DIV/0!</v>
+        <v>1064.235560477892</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -8838,15 +8835,15 @@
       </c>
       <c r="D33">
         <f>Riak!C37</f>
-        <v>2808</v>
+        <v>2765.3333333333335</v>
       </c>
       <c r="E33">
         <f>Aerospike!C37</f>
         <v>341.33333333333331</v>
       </c>
-      <c r="F33" t="e">
+      <c r="F33">
         <f>Memcached!C37</f>
-        <v>#DIV/0!</v>
+        <v>406.66666666666669</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -8859,15 +8856,15 @@
       </c>
       <c r="D34">
         <f>Riak!C38</f>
-        <v>122303</v>
+        <v>127231</v>
       </c>
       <c r="E34">
         <f>Aerospike!C38</f>
         <v>17132.333333333332</v>
       </c>
-      <c r="F34" t="e">
+      <c r="F34">
         <f>Memcached!C38</f>
-        <v>#DIV/0!</v>
+        <v>91625.666666666672</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -8880,15 +8877,15 @@
       </c>
       <c r="D35">
         <f>Riak!C39</f>
-        <v>8487</v>
+        <v>8903</v>
       </c>
       <c r="E35">
         <f>Aerospike!C39</f>
         <v>1197.6666666666667</v>
       </c>
-      <c r="F35" t="e">
+      <c r="F35">
         <f>Memcached!C39</f>
-        <v>#DIV/0!</v>
+        <v>1752.6666666666667</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -8901,15 +8898,15 @@
       </c>
       <c r="D36">
         <f>Riak!C40</f>
-        <v>13559</v>
+        <v>14495</v>
       </c>
       <c r="E36">
         <f>Aerospike!C40</f>
         <v>1779.6666666666667</v>
       </c>
-      <c r="F36" t="e">
+      <c r="F36">
         <f>Memcached!C40</f>
-        <v>#DIV/0!</v>
+        <v>2851</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -8931,7 +8928,7 @@
         <v>3</v>
       </c>
       <c r="F41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -8944,7 +8941,7 @@
       </c>
       <c r="D42">
         <f>Riak!C46</f>
-        <v>540018</v>
+        <v>562029.33333333337</v>
       </c>
       <c r="E42">
         <f>Aerospike!C46</f>
@@ -8965,7 +8962,7 @@
       </c>
       <c r="D43">
         <f>Riak!C47</f>
-        <v>1851.7901255143299</v>
+        <v>1783.3907950035066</v>
       </c>
       <c r="E43">
         <f>Aerospike!C47</f>
@@ -9010,7 +9007,7 @@
       </c>
       <c r="D45">
         <f>Riak!C49</f>
-        <v>2153.5019000000002</v>
+        <v>2241.0063320000004</v>
       </c>
       <c r="E45">
         <f>Aerospike!C49</f>
@@ -9031,7 +9028,7 @@
       </c>
       <c r="D46">
         <f>Riak!C50</f>
-        <v>811</v>
+        <v>804.66666666666663</v>
       </c>
       <c r="E46">
         <f>Aerospike!C50</f>
@@ -9052,7 +9049,7 @@
       </c>
       <c r="D47">
         <f>Riak!C51</f>
-        <v>64063</v>
+        <v>83903</v>
       </c>
       <c r="E47">
         <f>Aerospike!C51</f>
@@ -9073,7 +9070,7 @@
       </c>
       <c r="D48">
         <f>Riak!C52</f>
-        <v>3511</v>
+        <v>3714.3333333333335</v>
       </c>
       <c r="E48">
         <f>Aerospike!C52</f>
@@ -9094,7 +9091,7 @@
       </c>
       <c r="D49">
         <f>Riak!C53</f>
-        <v>6939</v>
+        <v>7885.666666666667</v>
       </c>
       <c r="E49">
         <f>Aerospike!C53</f>
@@ -9115,8 +9112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA6185-A47A-430A-AEC2-7ED0A4C5D4C7}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9869,8 +9866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8B41AC-D64A-4E90-ABED-E837F425F881}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9912,10 +9909,16 @@
       </c>
       <c r="C8">
         <f>AVERAGEA(D8:F8)</f>
-        <v>797604</v>
+        <v>803880.33333333337</v>
       </c>
       <c r="D8">
         <v>797604</v>
+      </c>
+      <c r="E8">
+        <v>980397</v>
+      </c>
+      <c r="F8">
+        <v>633640</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9924,10 +9927,16 @@
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C21" si="0">AVERAGEA(D9:F9)</f>
-        <v>1253.75499621366</v>
+        <v>1283.9777176479602</v>
       </c>
       <c r="D9">
         <v>1253.75499621366</v>
+      </c>
+      <c r="E9">
+        <v>1019.9949612248899</v>
+      </c>
+      <c r="F9">
+        <v>1578.1831955053301</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9944,6 +9953,12 @@
       <c r="D10">
         <v>500382</v>
       </c>
+      <c r="E10">
+        <v>499236</v>
+      </c>
+      <c r="F10">
+        <v>499886</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -9951,10 +9966,16 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>2054.67928302776</v>
+        <v>2175.8569730388999</v>
       </c>
       <c r="D11">
         <v>2054.67928302776</v>
+      </c>
+      <c r="E11">
+        <v>2529.8990737847398</v>
+      </c>
+      <c r="F11">
+        <v>1942.9925623042</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9963,10 +9984,16 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>858</v>
+        <v>861.33333333333337</v>
       </c>
       <c r="D12">
         <v>858</v>
+      </c>
+      <c r="E12">
+        <v>884</v>
+      </c>
+      <c r="F12">
+        <v>842</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9975,10 +10002,16 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>169855</v>
+        <v>158271</v>
       </c>
       <c r="D13">
         <v>169855</v>
+      </c>
+      <c r="E13">
+        <v>191103</v>
+      </c>
+      <c r="F13">
+        <v>113855</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9987,10 +10020,16 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>3311</v>
+        <v>3695</v>
       </c>
       <c r="D14">
         <v>3311</v>
+      </c>
+      <c r="E14">
+        <v>4803</v>
+      </c>
+      <c r="F14">
+        <v>2971</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9999,10 +10038,16 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>6375</v>
+        <v>7399</v>
       </c>
       <c r="D15">
         <v>6375</v>
+      </c>
+      <c r="E15">
+        <v>10151</v>
+      </c>
+      <c r="F15">
+        <v>5671</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -10019,6 +10064,12 @@
       <c r="D16">
         <v>499618</v>
       </c>
+      <c r="E16">
+        <v>500764</v>
+      </c>
+      <c r="F16">
+        <v>500114</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -10026,10 +10077,16 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>5649.6048753783698</v>
+        <v>5941.3298998398968</v>
       </c>
       <c r="D17">
         <v>5649.6048753783698</v>
+      </c>
+      <c r="E17">
+        <v>6813.1167181750297</v>
+      </c>
+      <c r="F17">
+        <v>5361.26810596629</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -10038,10 +10095,16 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>2528</v>
+        <v>2526.6666666666665</v>
       </c>
       <c r="D18">
         <v>2528</v>
+      </c>
+      <c r="E18">
+        <v>2626</v>
+      </c>
+      <c r="F18">
+        <v>2426</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -10050,10 +10113,16 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>176639</v>
+        <v>167764.33333333334</v>
       </c>
       <c r="D19">
         <v>176639</v>
+      </c>
+      <c r="E19">
+        <v>211199</v>
+      </c>
+      <c r="F19">
+        <v>115455</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -10062,10 +10131,16 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>8951</v>
+        <v>9819</v>
       </c>
       <c r="D20">
         <v>8951</v>
+      </c>
+      <c r="E20">
+        <v>12375</v>
+      </c>
+      <c r="F20">
+        <v>8131</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -10074,10 +10149,16 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>14215</v>
+        <v>16332.333333333334</v>
       </c>
       <c r="D21">
         <v>14215</v>
+      </c>
+      <c r="E21">
+        <v>21551</v>
+      </c>
+      <c r="F21">
+        <v>13231</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -10108,10 +10189,16 @@
       </c>
       <c r="C27">
         <f>AVERAGEA(D27:F27)</f>
-        <v>548477</v>
+        <v>562799.66666666663</v>
       </c>
       <c r="D27">
         <v>548477</v>
+      </c>
+      <c r="E27">
+        <v>555590</v>
+      </c>
+      <c r="F27">
+        <v>584332</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -10120,10 +10207,16 @@
       </c>
       <c r="C28">
         <f t="shared" ref="C28:C40" si="1">AVERAGEA(D28:F28)</f>
-        <v>1823.2305092100401</v>
+        <v>1778.1582630532967</v>
       </c>
       <c r="D28">
         <v>1823.2305092100401</v>
+      </c>
+      <c r="E28">
+        <v>1799.88840691877</v>
+      </c>
+      <c r="F28">
+        <v>1711.3558730310799</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -10140,6 +10233,12 @@
       <c r="D29">
         <v>949728</v>
       </c>
+      <c r="E29">
+        <v>949999</v>
+      </c>
+      <c r="F29">
+        <v>949933</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -10147,10 +10246,16 @@
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>2013.5313047525101</v>
+        <v>2072.9082253935767</v>
       </c>
       <c r="D30">
         <v>2013.5313047525101</v>
+      </c>
+      <c r="E30">
+        <v>2047.38028882135</v>
+      </c>
+      <c r="F30">
+        <v>2157.81308260687</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -10159,10 +10264,16 @@
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>852</v>
+        <v>825.33333333333337</v>
       </c>
       <c r="D31">
         <v>852</v>
+      </c>
+      <c r="E31">
+        <v>797</v>
+      </c>
+      <c r="F31">
+        <v>827</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -10171,10 +10282,16 @@
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>82303</v>
+        <v>110356.33333333333</v>
       </c>
       <c r="D32">
         <v>82303</v>
+      </c>
+      <c r="E32">
+        <v>124927</v>
+      </c>
+      <c r="F32">
+        <v>123839</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -10183,10 +10300,16 @@
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>3051</v>
+        <v>3232.3333333333335</v>
       </c>
       <c r="D33">
         <v>3051</v>
+      </c>
+      <c r="E33">
+        <v>3101</v>
+      </c>
+      <c r="F33">
+        <v>3545</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -10195,10 +10318,16 @@
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>6035</v>
+        <v>6805.666666666667</v>
       </c>
       <c r="D34">
         <v>6035</v>
+      </c>
+      <c r="E34">
+        <v>6755</v>
+      </c>
+      <c r="F34">
+        <v>7627</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -10208,12 +10337,18 @@
       <c r="B35" t="s">
         <v>16</v>
       </c>
-      <c r="C35" t="str">
+      <c r="C35">
         <f>D35</f>
-        <v>50 272</v>
-      </c>
-      <c r="D35" t="s">
-        <v>19</v>
+        <v>50272</v>
+      </c>
+      <c r="D35">
+        <v>50272</v>
+      </c>
+      <c r="E35">
+        <v>50001</v>
+      </c>
+      <c r="F35">
+        <v>50067</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -10222,10 +10357,16 @@
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>5714.9600163461901</v>
+        <v>5827.5136784126071</v>
       </c>
       <c r="D36">
         <v>5714.9600163461901</v>
+      </c>
+      <c r="E36">
+        <v>5720.7815662120502</v>
+      </c>
+      <c r="F36">
+        <v>6046.7994526795801</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -10234,10 +10375,16 @@
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>2808</v>
+        <v>2765.3333333333335</v>
       </c>
       <c r="D37">
         <v>2808</v>
+      </c>
+      <c r="E37">
+        <v>2678</v>
+      </c>
+      <c r="F37">
+        <v>2810</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -10246,10 +10393,16 @@
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>122303</v>
+        <v>127231</v>
       </c>
       <c r="D38">
         <v>122303</v>
+      </c>
+      <c r="E38">
+        <v>128383</v>
+      </c>
+      <c r="F38">
+        <v>131007</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -10258,10 +10411,16 @@
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>8487</v>
+        <v>8903</v>
       </c>
       <c r="D39">
         <v>8487</v>
+      </c>
+      <c r="E39">
+        <v>8455</v>
+      </c>
+      <c r="F39">
+        <v>9767</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -10270,10 +10429,16 @@
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>13559</v>
+        <v>14495</v>
       </c>
       <c r="D40">
         <v>13559</v>
+      </c>
+      <c r="E40">
+        <v>13975</v>
+      </c>
+      <c r="F40">
+        <v>15951</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -10304,10 +10469,16 @@
       </c>
       <c r="C46">
         <f>AVERAGEA(D46:F46)</f>
-        <v>540018</v>
+        <v>562029.33333333337</v>
       </c>
       <c r="D46">
         <v>540018</v>
+      </c>
+      <c r="E46">
+        <v>600768</v>
+      </c>
+      <c r="F46">
+        <v>545302</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -10316,10 +10487,16 @@
       </c>
       <c r="C47">
         <f t="shared" ref="C47:C53" si="2">AVERAGEA(D47:F47)</f>
-        <v>1851.7901255143299</v>
+        <v>1783.3907950035066</v>
       </c>
       <c r="D47">
         <v>1851.7901255143299</v>
+      </c>
+      <c r="E47">
+        <v>1664.5360605092101</v>
+      </c>
+      <c r="F47">
+        <v>1833.84619898698</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -10336,65 +10513,101 @@
       <c r="D48">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>1000000</v>
+      </c>
+      <c r="F48">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>8</v>
       </c>
       <c r="C49">
         <f t="shared" si="2"/>
-        <v>2153.5019000000002</v>
+        <v>2241.0063320000004</v>
       </c>
       <c r="D49">
         <v>2153.5019000000002</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>2395.5996220000002</v>
+      </c>
+      <c r="F49">
+        <v>2173.9174739999999</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>10</v>
       </c>
       <c r="C50">
         <f t="shared" si="2"/>
-        <v>811</v>
+        <v>804.66666666666663</v>
       </c>
       <c r="D50">
         <v>811</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>799</v>
+      </c>
+      <c r="F50">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>11</v>
       </c>
       <c r="C51">
         <f t="shared" si="2"/>
-        <v>64063</v>
+        <v>83903</v>
       </c>
       <c r="D51">
         <v>64063</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>110655</v>
+      </c>
+      <c r="F51">
+        <v>76991</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>12</v>
       </c>
       <c r="C52">
         <f t="shared" si="2"/>
-        <v>3511</v>
+        <v>3714.3333333333335</v>
       </c>
       <c r="D52">
         <v>3511</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>4151</v>
+      </c>
+      <c r="F52">
+        <v>3481</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>13</v>
       </c>
       <c r="C53">
         <f t="shared" si="2"/>
-        <v>6939</v>
+        <v>7885.666666666667</v>
       </c>
       <c r="D53">
         <v>6939</v>
+      </c>
+      <c r="E53">
+        <v>8607</v>
+      </c>
+      <c r="F53">
+        <v>8111</v>
       </c>
     </row>
   </sheetData>
@@ -10406,8 +10619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDCD321-116C-4788-8C82-6E80CAB0FE5C}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11160,7 +11373,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11170,7 +11383,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -11479,18 +11692,36 @@
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27" t="e">
+      <c r="C27">
         <f>AVERAGEA(D27:F27)</f>
-        <v>#DIV/0!</v>
+        <v>263195.66666666669</v>
+      </c>
+      <c r="D27">
+        <v>310762</v>
+      </c>
+      <c r="E27">
+        <v>250843</v>
+      </c>
+      <c r="F27">
+        <v>227982</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>5</v>
       </c>
-      <c r="C28" t="e">
+      <c r="C28">
         <f t="shared" ref="C28:C40" si="1">AVERAGEA(D28:F28)</f>
-        <v>#DIV/0!</v>
+        <v>3863.5883942419064</v>
+      </c>
+      <c r="D28">
+        <v>3217.8966540310498</v>
+      </c>
+      <c r="E28">
+        <v>3986.5573286876602</v>
+      </c>
+      <c r="F28">
+        <v>4386.3112000070096</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -11502,52 +11733,106 @@
       </c>
       <c r="C29">
         <f>D29</f>
-        <v>0</v>
+        <v>950435</v>
+      </c>
+      <c r="D29">
+        <v>950435</v>
+      </c>
+      <c r="E29">
+        <v>949527</v>
+      </c>
+      <c r="F29">
+        <v>949927</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>8</v>
       </c>
-      <c r="C30" t="e">
+      <c r="C30">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1046.1802303928137</v>
+      </c>
+      <c r="D30">
+        <v>1235.2323725452</v>
+      </c>
+      <c r="E30">
+        <v>997.01798579713898</v>
+      </c>
+      <c r="F30">
+        <v>906.29033283610204</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>10</v>
       </c>
-      <c r="C31" t="e">
+      <c r="C31">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>389</v>
+      </c>
+      <c r="D31">
+        <v>395</v>
+      </c>
+      <c r="E31">
+        <v>389</v>
+      </c>
+      <c r="F31">
+        <v>383</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="C32" t="e">
+      <c r="C32">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>112020.33333333333</v>
+      </c>
+      <c r="D32">
+        <v>179839</v>
+      </c>
+      <c r="E32">
+        <v>86655</v>
+      </c>
+      <c r="F32">
+        <v>69567</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>12</v>
       </c>
-      <c r="C33" t="e">
+      <c r="C33">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1735.3333333333333</v>
+      </c>
+      <c r="D33">
+        <v>2363</v>
+      </c>
+      <c r="E33">
+        <v>1562</v>
+      </c>
+      <c r="F33">
+        <v>1281</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>13</v>
       </c>
-      <c r="C34" t="e">
+      <c r="C34">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2813</v>
+      </c>
+      <c r="D34">
+        <v>4235</v>
+      </c>
+      <c r="E34">
+        <v>2439</v>
+      </c>
+      <c r="F34">
+        <v>1765</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -11559,52 +11844,106 @@
       </c>
       <c r="C35">
         <f>D35</f>
-        <v>0</v>
+        <v>49565</v>
+      </c>
+      <c r="D35">
+        <v>49565</v>
+      </c>
+      <c r="E35">
+        <v>50473</v>
+      </c>
+      <c r="F35">
+        <v>50073</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>8</v>
       </c>
-      <c r="C36" t="e">
+      <c r="C36">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1064.235560477892</v>
+      </c>
+      <c r="D36">
+        <v>1256.08639160698</v>
+      </c>
+      <c r="E36">
+        <v>1020.0730687694401</v>
+      </c>
+      <c r="F36">
+        <v>916.54722105725602</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>10</v>
       </c>
-      <c r="C37" t="e">
+      <c r="C37">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>406.66666666666669</v>
+      </c>
+      <c r="D37">
+        <v>444</v>
+      </c>
+      <c r="E37">
+        <v>393</v>
+      </c>
+      <c r="F37">
+        <v>383</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>11</v>
       </c>
-      <c r="C38" t="e">
+      <c r="C38">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>91625.666666666672</v>
+      </c>
+      <c r="D38">
+        <v>128063</v>
+      </c>
+      <c r="E38">
+        <v>77247</v>
+      </c>
+      <c r="F38">
+        <v>69567</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>12</v>
       </c>
-      <c r="C39" t="e">
+      <c r="C39">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1752.6666666666667</v>
+      </c>
+      <c r="D39">
+        <v>2383</v>
+      </c>
+      <c r="E39">
+        <v>1594</v>
+      </c>
+      <c r="F39">
+        <v>1281</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>13</v>
       </c>
-      <c r="C40" t="e">
+      <c r="C40">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2851</v>
+      </c>
+      <c r="D40">
+        <v>4271</v>
+      </c>
+      <c r="E40">
+        <v>2517</v>
+      </c>
+      <c r="F40">
+        <v>1765</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
wiki citace změna, oprava chyb v části textu, template grafů
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA13244-E514-493E-AEED-19D5EE644B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0D5DDB-E287-4F31-9027-CB0EBFE13BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workloads - data" sheetId="1" r:id="rId1"/>
@@ -8298,7 +8298,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Testing Insert times + Average Read/Write times for beeing one information
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0D5DDB-E287-4F31-9027-CB0EBFE13BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BEDA29-A853-4DA2-BD0D-658911E140AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Workloads - data" sheetId="1" r:id="rId1"/>
-    <sheet name="Redis" sheetId="2" r:id="rId2"/>
-    <sheet name="Riak" sheetId="3" r:id="rId3"/>
-    <sheet name="Aerospike" sheetId="4" r:id="rId4"/>
-    <sheet name="Memcached" sheetId="5" r:id="rId5"/>
+    <sheet name="Workloads - Read,Write" sheetId="1" r:id="rId1"/>
+    <sheet name="Workloads - Insert" sheetId="6" r:id="rId2"/>
+    <sheet name="Redis" sheetId="2" r:id="rId3"/>
+    <sheet name="Riak" sheetId="3" r:id="rId4"/>
+    <sheet name="Aerospike" sheetId="4" r:id="rId5"/>
+    <sheet name="Memcached" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="24">
   <si>
     <t>DB</t>
   </si>
@@ -100,6 +101,18 @@
   </si>
   <si>
     <t>Memcached</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>R+W</t>
+  </si>
+  <si>
+    <t>1211.4163880408973</t>
+  </si>
+  <si>
+    <t>Average Insert - Workloads A, B, C</t>
   </si>
 </sst>
 </file>
@@ -210,7 +223,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$16</c:f>
+              <c:f>'Workloads - Read,Write'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -231,7 +244,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - data'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -251,7 +264,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$16:$F$16</c:f>
+              <c:f>'Workloads - Read,Write'!$C$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -504,7 +517,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$17</c:f>
+              <c:f>'Workloads - Read,Write'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -525,7 +538,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - data'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -545,7 +558,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$17:$F$17</c:f>
+              <c:f>'Workloads - Read,Write'!$C$17:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -798,7 +811,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$16</c:f>
+              <c:f>'Workloads - Read,Write'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -819,7 +832,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Workloads - data'!$C$3:$E$3,'Workloads - data'!$F$3)</c:f>
+              <c:f>('Workloads - Read,Write'!$C$3:$E$3,'Workloads - Read,Write'!$F$3)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -839,7 +852,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$35:$F$35</c:f>
+              <c:f>'Workloads - Read,Write'!$C$41:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1092,7 +1105,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$17</c:f>
+              <c:f>'Workloads - Read,Write'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1113,7 +1126,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Workloads - data'!$C$3:$E$3,'Workloads - data'!$F$3)</c:f>
+              <c:f>('Workloads - Read,Write'!$C$3:$E$3,'Workloads - Read,Write'!$F$3)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1133,7 +1146,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$36:$F$36</c:f>
+              <c:f>'Workloads - Read,Write'!$C$42:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1386,7 +1399,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$16</c:f>
+              <c:f>'Workloads - Read,Write'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1407,7 +1420,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Workloads - data'!$C$3:$E$3,'Workloads - data'!$F$3)</c:f>
+              <c:f>('Workloads - Read,Write'!$C$3:$E$3,'Workloads - Read,Write'!$F$3)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1427,7 +1440,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$48:$F$48</c:f>
+              <c:f>'Workloads - Read,Write'!$C$60:$F$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1680,7 +1693,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$17</c:f>
+              <c:f>'Workloads - Read,Write'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1701,7 +1714,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - data'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1721,7 +1734,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$49:$F$49</c:f>
+              <c:f>'Workloads - Read,Write'!$C$61:$F$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1974,7 +1987,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$5</c:f>
+              <c:f>'Workloads - Read,Write'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1995,7 +2008,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - data'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2015,7 +2028,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$5:$F$5</c:f>
+              <c:f>'Workloads - Read,Write'!$C$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2268,7 +2281,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$5</c:f>
+              <c:f>'Workloads - Read,Write'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2289,7 +2302,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Workloads - data'!$C$3:$E$3,'Workloads - data'!$F$3)</c:f>
+              <c:f>('Workloads - Read,Write'!$C$3:$E$3,'Workloads - Read,Write'!$F$3)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2309,7 +2322,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$24:$F$24</c:f>
+              <c:f>'Workloads - Read,Write'!$C$30:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2562,7 +2575,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - data'!$B$5</c:f>
+              <c:f>'Workloads - Read,Write'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2583,7 +2596,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - data'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2603,7 +2616,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - data'!$C$43:$F$43</c:f>
+              <c:f>'Workloads - Read,Write'!$C$55:$F$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -7692,15 +7705,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7735,7 +7748,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7767,13 +7780,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7805,13 +7818,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7843,13 +7856,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7881,13 +7894,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7925,7 +7938,7 @@
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7957,13 +7970,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7995,13 +8008,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8295,10 +8308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8629,221 +8642,217 @@
         <v>1850.6666666666667</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>1500000</v>
+      </c>
+      <c r="D18">
+        <v>1000000</v>
+      </c>
+      <c r="E18">
+        <v>1000000</v>
+      </c>
+      <c r="F18">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <f>AVERAGEA(C7,C13)</f>
+        <v>830.44716603206803</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:F19" si="0">AVERAGEA(D7,D13)</f>
+        <v>4058.5934364393984</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>784.27154740916467</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>967.90285344364963</v>
+      </c>
+    </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <f>AVERAGEA(C8,C14)</f>
+        <v>315.16666666666663</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:F20" si="1">AVERAGEA(D8,D14)</f>
+        <v>1694</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>317</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>401.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <f>AVERAGEA(C9,C15)</f>
+        <v>47924.333333333328</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:F21" si="2">AVERAGEA(D9,D15)</f>
+        <v>163017.66666666669</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>28532.333333333336</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>82713.666666666672</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <f>AVERAGEA(C10,C16)</f>
+        <v>1273</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22:F22" si="3">AVERAGEA(D10,D16)</f>
+        <v>6757</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>1121.8333333333335</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>1386.3333333333335</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <f>AVERAGEA(C11,C17)</f>
+        <v>1904.5</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:F23" si="4">AVERAGEA(D11,D17)</f>
+        <v>11865.666666666668</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
+        <v>1539.3333333333333</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>1848.3333333333335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C23">
+      <c r="C29">
         <f>Redis!C27</f>
         <v>212026.33333333334</v>
       </c>
-      <c r="D23">
+      <c r="D29">
         <f>Riak!C27</f>
         <v>562799.66666666663</v>
       </c>
-      <c r="E23">
+      <c r="E29">
         <f>Aerospike!C27</f>
         <v>202264</v>
       </c>
-      <c r="F23">
+      <c r="F29">
         <f>Memcached!C27</f>
         <v>263195.66666666669</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>5</v>
       </c>
-      <c r="C24">
+      <c r="C30">
         <f>Redis!C28</f>
         <v>4726.9578685717897</v>
       </c>
-      <c r="D24">
+      <c r="D30">
         <f>Riak!C28</f>
         <v>1778.1582630532967</v>
       </c>
-      <c r="E24">
+      <c r="E30">
         <f>Aerospike!C28</f>
         <v>4945.3776482559506</v>
       </c>
-      <c r="F24">
+      <c r="F30">
         <f>Memcached!C28</f>
         <v>3863.5883942419064</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B31" t="s">
         <v>16</v>
       </c>
-      <c r="C25">
+      <c r="C31">
         <f>Redis!C29</f>
         <v>949836</v>
       </c>
-      <c r="D25">
+      <c r="D31">
         <f>Riak!C29</f>
         <v>949728</v>
       </c>
-      <c r="E25">
+      <c r="E31">
         <f>Aerospike!C29</f>
         <v>949706</v>
       </c>
-      <c r="F25">
+      <c r="F31">
         <f>Memcached!C29</f>
         <v>950435</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26">
-        <f>Redis!C30</f>
-        <v>845.21823030995529</v>
-      </c>
-      <c r="D26">
-        <f>Riak!C30</f>
-        <v>2072.9082253935767</v>
-      </c>
-      <c r="E26">
-        <f>Aerospike!C30</f>
-        <v>805.96629449109275</v>
-      </c>
-      <c r="F26">
-        <f>Memcached!C30</f>
-        <v>1046.1802303928137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27">
-        <f>Redis!C31</f>
-        <v>313.66666666666669</v>
-      </c>
-      <c r="D27">
-        <f>Riak!C31</f>
-        <v>825.33333333333337</v>
-      </c>
-      <c r="E27">
-        <f>Aerospike!C31</f>
-        <v>313.33333333333331</v>
-      </c>
-      <c r="F27">
-        <f>Memcached!C31</f>
-        <v>389</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28">
-        <f>Redis!C32</f>
-        <v>50559</v>
-      </c>
-      <c r="D28">
-        <f>Riak!C32</f>
-        <v>110356.33333333333</v>
-      </c>
-      <c r="E28">
-        <f>Aerospike!C32</f>
-        <v>25732.333333333332</v>
-      </c>
-      <c r="F28">
-        <f>Memcached!C32</f>
-        <v>112020.33333333333</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29">
-        <f>Redis!C33</f>
-        <v>1325</v>
-      </c>
-      <c r="D29">
-        <f>Riak!C33</f>
-        <v>3232.3333333333335</v>
-      </c>
-      <c r="E29">
-        <f>Aerospike!C33</f>
-        <v>1188</v>
-      </c>
-      <c r="F29">
-        <f>Memcached!C33</f>
-        <v>1735.3333333333333</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30">
-        <f>Redis!C34</f>
-        <v>2232.3333333333335</v>
-      </c>
-      <c r="D30">
-        <f>Riak!C34</f>
-        <v>6805.666666666667</v>
-      </c>
-      <c r="E30">
-        <f>Aerospike!C34</f>
-        <v>1756</v>
-      </c>
-      <c r="F30">
-        <f>Memcached!C34</f>
-        <v>2813</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31">
-        <f>Redis!C35</f>
-        <v>50164</v>
-      </c>
-      <c r="D31">
-        <f>Riak!C35</f>
-        <v>50272</v>
-      </c>
-      <c r="E31">
-        <f>Aerospike!C35</f>
-        <v>50294</v>
-      </c>
-      <c r="F31">
-        <f>Memcached!C35</f>
-        <v>49565</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -8851,20 +8860,20 @@
         <v>8</v>
       </c>
       <c r="C32">
-        <f>Redis!C36</f>
-        <v>841.38027581715448</v>
+        <f>Redis!C30</f>
+        <v>845.21823030995529</v>
       </c>
       <c r="D32">
-        <f>Riak!C36</f>
-        <v>5827.5136784126071</v>
+        <f>Riak!C30</f>
+        <v>2072.9082253935767</v>
       </c>
       <c r="E32">
-        <f>Aerospike!C36</f>
-        <v>809.97773750073532</v>
+        <f>Aerospike!C30</f>
+        <v>805.96629449109275</v>
       </c>
       <c r="F32">
-        <f>Memcached!C36</f>
-        <v>1064.235560477892</v>
+        <f>Memcached!C30</f>
+        <v>1046.1802303928137</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -8872,20 +8881,20 @@
         <v>10</v>
       </c>
       <c r="C33">
-        <f>Redis!C37</f>
-        <v>342</v>
+        <f>Redis!C31</f>
+        <v>313.66666666666669</v>
       </c>
       <c r="D33">
-        <f>Riak!C37</f>
-        <v>2765.3333333333335</v>
+        <f>Riak!C31</f>
+        <v>825.33333333333337</v>
       </c>
       <c r="E33">
-        <f>Aerospike!C37</f>
-        <v>341.33333333333331</v>
+        <f>Aerospike!C31</f>
+        <v>313.33333333333331</v>
       </c>
       <c r="F33">
-        <f>Memcached!C37</f>
-        <v>406.66666666666669</v>
+        <f>Memcached!C31</f>
+        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -8893,20 +8902,20 @@
         <v>11</v>
       </c>
       <c r="C34">
-        <f>Redis!C38</f>
-        <v>41449.666666666664</v>
+        <f>Redis!C32</f>
+        <v>50559</v>
       </c>
       <c r="D34">
-        <f>Riak!C38</f>
-        <v>127231</v>
+        <f>Riak!C32</f>
+        <v>110356.33333333333</v>
       </c>
       <c r="E34">
-        <f>Aerospike!C38</f>
-        <v>17132.333333333332</v>
+        <f>Aerospike!C32</f>
+        <v>25732.333333333332</v>
       </c>
       <c r="F34">
-        <f>Memcached!C38</f>
-        <v>91625.666666666672</v>
+        <f>Memcached!C32</f>
+        <v>112020.33333333333</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -8914,20 +8923,20 @@
         <v>12</v>
       </c>
       <c r="C35">
-        <f>Redis!C39</f>
-        <v>1322.3333333333333</v>
+        <f>Redis!C33</f>
+        <v>1325</v>
       </c>
       <c r="D35">
-        <f>Riak!C39</f>
-        <v>8903</v>
+        <f>Riak!C33</f>
+        <v>3232.3333333333335</v>
       </c>
       <c r="E35">
-        <f>Aerospike!C39</f>
-        <v>1197.6666666666667</v>
+        <f>Aerospike!C33</f>
+        <v>1188</v>
       </c>
       <c r="F35">
-        <f>Memcached!C39</f>
-        <v>1752.6666666666667</v>
+        <f>Memcached!C33</f>
+        <v>1735.3333333333333</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -8935,211 +8944,465 @@
         <v>13</v>
       </c>
       <c r="C36">
+        <f>Redis!C34</f>
+        <v>2232.3333333333335</v>
+      </c>
+      <c r="D36">
+        <f>Riak!C34</f>
+        <v>6805.666666666667</v>
+      </c>
+      <c r="E36">
+        <f>Aerospike!C34</f>
+        <v>1756</v>
+      </c>
+      <c r="F36">
+        <f>Memcached!C34</f>
+        <v>2813</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <f>Redis!C35</f>
+        <v>50164</v>
+      </c>
+      <c r="D37">
+        <f>Riak!C35</f>
+        <v>50272</v>
+      </c>
+      <c r="E37">
+        <f>Aerospike!C35</f>
+        <v>50294</v>
+      </c>
+      <c r="F37">
+        <f>Memcached!C35</f>
+        <v>49565</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <f>Redis!C36</f>
+        <v>841.38027581715448</v>
+      </c>
+      <c r="D38">
+        <f>Riak!C36</f>
+        <v>5827.5136784126071</v>
+      </c>
+      <c r="E38">
+        <f>Aerospike!C36</f>
+        <v>809.97773750073532</v>
+      </c>
+      <c r="F38">
+        <f>Memcached!C36</f>
+        <v>1064.235560477892</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <f>Redis!C37</f>
+        <v>342</v>
+      </c>
+      <c r="D39">
+        <f>Riak!C37</f>
+        <v>2765.3333333333335</v>
+      </c>
+      <c r="E39">
+        <f>Aerospike!C37</f>
+        <v>341.33333333333331</v>
+      </c>
+      <c r="F39">
+        <f>Memcached!C37</f>
+        <v>406.66666666666669</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <f>Redis!C38</f>
+        <v>41449.666666666664</v>
+      </c>
+      <c r="D40">
+        <f>Riak!C38</f>
+        <v>127231</v>
+      </c>
+      <c r="E40">
+        <f>Aerospike!C38</f>
+        <v>17132.333333333332</v>
+      </c>
+      <c r="F40">
+        <f>Memcached!C38</f>
+        <v>91625.666666666672</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <f>Redis!C39</f>
+        <v>1322.3333333333333</v>
+      </c>
+      <c r="D41">
+        <f>Riak!C39</f>
+        <v>8903</v>
+      </c>
+      <c r="E41">
+        <f>Aerospike!C39</f>
+        <v>1197.6666666666667</v>
+      </c>
+      <c r="F41">
+        <f>Memcached!C39</f>
+        <v>1752.6666666666667</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42">
         <f>Redis!C40</f>
         <v>2243.3333333333335</v>
       </c>
-      <c r="D36">
+      <c r="D42">
         <f>Riak!C40</f>
         <v>14495</v>
       </c>
-      <c r="E36">
+      <c r="E42">
         <f>Aerospike!C40</f>
         <v>1779.6666666666667</v>
       </c>
-      <c r="F36">
+      <c r="F42">
         <f>Memcached!C40</f>
         <v>2851</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <v>1000000</v>
+      </c>
+      <c r="D43">
+        <v>1000000</v>
+      </c>
+      <c r="E43">
+        <v>1000000</v>
+      </c>
+      <c r="F43">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <f>AVERAGEA(C32,C38)</f>
+        <v>843.29925306355494</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ref="D44:F44" si="5">AVERAGEA(D32,D38)</f>
+        <v>3950.2109519030919</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="5"/>
+        <v>807.97201599591403</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="5"/>
+        <v>1055.2078954353528</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ref="C45:F48" si="6">AVERAGEA(C33,C39)</f>
+        <v>327.83333333333337</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="6"/>
+        <v>1795.3333333333335</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="6"/>
+        <v>327.33333333333331</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="6"/>
+        <v>397.83333333333337</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="6"/>
+        <v>46004.333333333328</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="6"/>
+        <v>118793.66666666666</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="6"/>
+        <v>21432.333333333332</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="6"/>
+        <v>101823</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="6"/>
+        <v>1323.6666666666665</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="6"/>
+        <v>6067.666666666667</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="6"/>
+        <v>1192.8333333333335</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="6"/>
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="6"/>
+        <v>2237.8333333333335</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="6"/>
+        <v>10650.333333333334</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>1767.8333333333335</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="6"/>
+        <v>2832</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>0</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C53" t="s">
         <v>1</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D53" t="s">
         <v>2</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E53" t="s">
         <v>3</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F53" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>4</v>
       </c>
-      <c r="C42">
+      <c r="C54">
         <f>Redis!C46</f>
         <v>205492.66666666666</v>
       </c>
-      <c r="D42">
+      <c r="D54">
         <f>Riak!C46</f>
         <v>562029.33333333337</v>
       </c>
-      <c r="E42">
+      <c r="E54">
         <f>Aerospike!C46</f>
         <v>209528</v>
       </c>
-      <c r="F42">
+      <c r="F54">
         <f>Memcached!C46</f>
         <v>221353.33333333334</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>5</v>
       </c>
-      <c r="C43">
+      <c r="C55">
         <f>Redis!C47</f>
         <v>4868.3014319549338</v>
       </c>
-      <c r="D43">
+      <c r="D55">
         <f>Riak!C47</f>
         <v>1783.3907950035066</v>
       </c>
-      <c r="E43">
+      <c r="E55">
         <f>Aerospike!C47</f>
         <v>4778.1274961757899</v>
       </c>
-      <c r="F43">
+      <c r="F55">
         <f>Memcached!C47</f>
         <v>4517.6713328397063</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>9</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B56" t="s">
         <v>16</v>
       </c>
-      <c r="C44">
+      <c r="C56">
         <f>Redis!C48</f>
         <v>1000000</v>
       </c>
-      <c r="D44">
+      <c r="D56">
         <f>Riak!C48</f>
         <v>1000000</v>
       </c>
-      <c r="E44">
+      <c r="E56">
         <f>Aerospike!C48</f>
         <v>1000000</v>
       </c>
-      <c r="F44">
+      <c r="F56">
         <f>Memcached!C48</f>
         <v>1000000</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>8</v>
       </c>
-      <c r="C45">
+      <c r="C57">
         <f>Redis!C49</f>
         <v>819.3226933333334</v>
       </c>
-      <c r="D45">
+      <c r="D57">
         <f>Riak!C49</f>
         <v>2241.0063320000004</v>
       </c>
-      <c r="E45">
+      <c r="E57">
         <f>Aerospike!C49</f>
         <v>835.167418</v>
       </c>
-      <c r="F45">
+      <c r="F57">
         <f>Memcached!C49</f>
         <v>880.1736556666666</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C46">
+      <c r="C58">
         <f>Redis!C50</f>
         <v>308.66666666666669</v>
       </c>
-      <c r="D46">
+      <c r="D58">
         <f>Riak!C50</f>
         <v>804.66666666666663</v>
       </c>
-      <c r="E46">
+      <c r="E58">
         <f>Aerospike!C50</f>
         <v>319.33333333333331</v>
       </c>
-      <c r="F46">
+      <c r="F58">
         <f>Memcached!C50</f>
         <v>376</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="C47">
+      <c r="C59">
         <f>Redis!C51</f>
         <v>33935</v>
       </c>
-      <c r="D47">
+      <c r="D59">
         <f>Riak!C51</f>
         <v>83903</v>
       </c>
-      <c r="E47">
+      <c r="E59">
         <f>Aerospike!C51</f>
         <v>41881.666666666664</v>
       </c>
-      <c r="F47">
+      <c r="F59">
         <f>Memcached!C51</f>
         <v>39071</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>12</v>
       </c>
-      <c r="C48">
+      <c r="C60">
         <f>Redis!C52</f>
         <v>1213.3333333333333</v>
       </c>
-      <c r="D48">
+      <c r="D60">
         <f>Riak!C52</f>
         <v>3714.3333333333335</v>
       </c>
-      <c r="E48">
+      <c r="E60">
         <f>Aerospike!C52</f>
         <v>1242.3333333333333</v>
       </c>
-      <c r="F48">
+      <c r="F60">
         <f>Memcached!C52</f>
         <v>1233.3333333333333</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>13</v>
       </c>
-      <c r="C49">
+      <c r="C61">
         <f>Redis!C53</f>
         <v>1856</v>
       </c>
-      <c r="D49">
+      <c r="D61">
         <f>Riak!C53</f>
         <v>7885.666666666667</v>
       </c>
-      <c r="E49">
+      <c r="E61">
         <f>Aerospike!C53</f>
         <v>1861.6666666666667</v>
       </c>
-      <c r="F49">
+      <c r="F61">
         <f>Memcached!C53</f>
         <v>1615.3333333333333</v>
       </c>
@@ -9151,6 +9414,704 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E628E191-458C-48C1-BA88-DA60FE101777}">
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>38866</v>
+      </c>
+      <c r="D4">
+        <v>82548</v>
+      </c>
+      <c r="E4">
+        <v>19436</v>
+      </c>
+      <c r="F4">
+        <v>25485</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2572.9429321257599</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>5145.0915826301698</v>
+      </c>
+      <c r="F5">
+        <v>3923.87679026878</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>100000</v>
+      </c>
+      <c r="D6">
+        <v>100000</v>
+      </c>
+      <c r="E6">
+        <v>100000</v>
+      </c>
+      <c r="F6">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1546.5329300000001</v>
+      </c>
+      <c r="D7">
+        <v>3260.0788400000001</v>
+      </c>
+      <c r="E7">
+        <v>768.75090999999998</v>
+      </c>
+      <c r="F7">
+        <v>980.03053</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>758</v>
+      </c>
+      <c r="D8">
+        <v>1164</v>
+      </c>
+      <c r="E8">
+        <v>315</v>
+      </c>
+      <c r="F8">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>33535</v>
+      </c>
+      <c r="D9">
+        <v>403967</v>
+      </c>
+      <c r="E9">
+        <v>65983</v>
+      </c>
+      <c r="F9">
+        <v>49951</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>2205</v>
+      </c>
+      <c r="D10">
+        <v>6127</v>
+      </c>
+      <c r="E10">
+        <v>1096</v>
+      </c>
+      <c r="F10">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>3033</v>
+      </c>
+      <c r="D11">
+        <v>11855</v>
+      </c>
+      <c r="E11">
+        <v>1492</v>
+      </c>
+      <c r="F11">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>38448</v>
+      </c>
+      <c r="D17">
+        <v>63834</v>
+      </c>
+      <c r="E17">
+        <v>21084</v>
+      </c>
+      <c r="F17">
+        <v>26219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>2600.9155222638301</v>
+      </c>
+      <c r="D18">
+        <v>1566.5632734906101</v>
+      </c>
+      <c r="E18">
+        <v>4742.9330297856104</v>
+      </c>
+      <c r="F18">
+        <v>3814.02799496548</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>100000</v>
+      </c>
+      <c r="D19">
+        <v>100000</v>
+      </c>
+      <c r="E19">
+        <v>100000</v>
+      </c>
+      <c r="F19">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>1530.1638800000001</v>
+      </c>
+      <c r="D20">
+        <v>2521.18208</v>
+      </c>
+      <c r="E20">
+        <v>835.85717</v>
+      </c>
+      <c r="F20">
+        <v>1018.51215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>749</v>
+      </c>
+      <c r="D21">
+        <v>1083</v>
+      </c>
+      <c r="E21">
+        <v>325</v>
+      </c>
+      <c r="F21">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>16215</v>
+      </c>
+      <c r="D22">
+        <v>234751</v>
+      </c>
+      <c r="E22">
+        <v>24479</v>
+      </c>
+      <c r="F22">
+        <v>66623</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>2123</v>
+      </c>
+      <c r="D23">
+        <v>3541</v>
+      </c>
+      <c r="E23">
+        <v>1300</v>
+      </c>
+      <c r="F23">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>3151</v>
+      </c>
+      <c r="D24">
+        <v>6315</v>
+      </c>
+      <c r="E24">
+        <v>1906</v>
+      </c>
+      <c r="F24">
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>40238</v>
+      </c>
+      <c r="D30">
+        <v>62865</v>
+      </c>
+      <c r="E30">
+        <v>20116</v>
+      </c>
+      <c r="F30">
+        <v>24534</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>2485.2129827526201</v>
+      </c>
+      <c r="D31">
+        <v>1590.7102521275699</v>
+      </c>
+      <c r="E31">
+        <v>4971.1672300656101</v>
+      </c>
+      <c r="F31">
+        <v>4075.9761962990101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>100000</v>
+      </c>
+      <c r="D32">
+        <v>100000</v>
+      </c>
+      <c r="E32">
+        <v>100000</v>
+      </c>
+      <c r="F32">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>1602.16408</v>
+      </c>
+      <c r="D33">
+        <v>2480.51809</v>
+      </c>
+      <c r="E33">
+        <v>797.11816999999996</v>
+      </c>
+      <c r="F33">
+        <v>952.01183000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>779</v>
+      </c>
+      <c r="D34">
+        <v>1117</v>
+      </c>
+      <c r="E34">
+        <v>316</v>
+      </c>
+      <c r="F34">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>20031</v>
+      </c>
+      <c r="D35">
+        <v>338943</v>
+      </c>
+      <c r="E35">
+        <v>14319</v>
+      </c>
+      <c r="F35">
+        <v>95359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>2329</v>
+      </c>
+      <c r="D36">
+        <v>3491</v>
+      </c>
+      <c r="E36">
+        <v>1202</v>
+      </c>
+      <c r="F36">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>3401</v>
+      </c>
+      <c r="D37">
+        <v>6203</v>
+      </c>
+      <c r="E37">
+        <v>1672</v>
+      </c>
+      <c r="F37">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <f>AVERAGEA(C4,C17,C30)</f>
+        <v>39184</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ref="D43:F45" si="0">AVERAGEA(D4,D17,D30)</f>
+        <v>69749</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>20212</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>25412.666666666668</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <f>AVERAGEA(C5,C18,C31)</f>
+        <v>2553.0238123807371</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>1052.4245085393934</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>4953.0639474937971</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>3937.9603271777564</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45">
+        <f>AVERAGEA(C6,C19,C32)</f>
+        <v>100000</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:F46" si="1">AVERAGEA(C7,C20,C33)</f>
+        <v>1559.6202966666667</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>2753.9263366666669</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>800.57541666666657</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>983.51816999999994</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:F47" si="2">AVERAGEA(C8,C21,C34)</f>
+        <v>762</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>1121.3333333333333</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>318.66666666666669</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
+        <v>406.33333333333331</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48:F48" si="3">AVERAGEA(C9,C22,C35)</f>
+        <v>23260.333333333332</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="3"/>
+        <v>325887</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="3"/>
+        <v>34927</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="3"/>
+        <v>70644.333333333328</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:F49" si="4">AVERAGEA(C10,C23,C36)</f>
+        <v>2219</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="4"/>
+        <v>4386.333333333333</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="4"/>
+        <v>1199.3333333333333</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="4"/>
+        <v>1536.6666666666667</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ref="C50:F50" si="5">AVERAGEA(C11,C24,C37)</f>
+        <v>3195</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="5"/>
+        <v>8124.333333333333</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="5"/>
+        <v>1690</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="5"/>
+        <v>2322.3333333333335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA6185-A47A-430A-AEC2-7ED0A4C5D4C7}">
   <dimension ref="A1:F53"/>
   <sheetViews>
@@ -9904,7 +10865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8B41AC-D64A-4E90-ABED-E837F425F881}">
   <dimension ref="A1:F53"/>
   <sheetViews>
@@ -10657,7 +11618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDCD321-116C-4788-8C82-6E80CAB0FE5C}">
   <dimension ref="A1:F53"/>
   <sheetViews>
@@ -11410,7 +12371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C80EE16-73D0-4778-A1BC-D419AAA6A283}">
   <dimension ref="A1:F53"/>
   <sheetViews>

</xml_diff>

<commit_message>
grafy Percentile 95/99% Workloads A - C
- todo ostatní grafy
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BEDA29-A853-4DA2-BD0D-658911E140AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D47B49-51DD-4ECD-BD68-FF0E2514F0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workloads - Read,Write" sheetId="1" r:id="rId1"/>
@@ -8310,8 +8310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8755,11 +8755,11 @@
         <v>1904.5</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:F23" si="4">AVERAGEA(D11,D17)</f>
+        <f>AVERAGEA(D11,D17)</f>
         <v>11865.666666666668</v>
       </c>
       <c r="E23">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D23:F23" si="4">AVERAGEA(E11,E17)</f>
         <v>1539.3333333333333</v>
       </c>
       <c r="F23">
@@ -9417,7 +9417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E628E191-458C-48C1-BA88-DA60FE101777}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Testový scénář 2 - Workload B
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4BFD91-47E5-4DA3-A0EE-1E390E56F833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F592B4-B485-40A7-92C8-A4B3E7EACF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10940,8 +10940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13500,7 +13500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8B41AC-D64A-4E90-ABED-E837F425F881}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -14253,8 +14253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDCD321-116C-4788-8C82-6E80CAB0FE5C}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tabulka Testový scénář 4 - Insert only
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F592B4-B485-40A7-92C8-A4B3E7EACF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4219637-4679-452B-BF28-5AA5F8A866B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workloads - Read,Write" sheetId="1" r:id="rId1"/>
@@ -10940,7 +10940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
@@ -12047,8 +12047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E628E191-458C-48C1-BA88-DA60FE101777}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Testový scénář 3 - Workload C + Testový scénář 4 - Insert only
</commit_message>
<xml_diff>
--- a/Tests/DB Tests.xlsx
+++ b/Tests/DB Tests.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDD_VSB\Git VŠB - StandAlones\DP-KVDBS\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4219637-4679-452B-BF28-5AA5F8A866B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFCC48D-2F1E-47F3-82AC-E94EA0EA3BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Workloads - Read,Write" sheetId="1" r:id="rId1"/>
+    <sheet name="Workloads - Read, Update" sheetId="1" r:id="rId1"/>
     <sheet name="Workloads - Insert" sheetId="6" r:id="rId2"/>
     <sheet name="Redis" sheetId="2" r:id="rId3"/>
-    <sheet name="Riak" sheetId="3" r:id="rId4"/>
+    <sheet name="Riak KV" sheetId="3" r:id="rId4"/>
     <sheet name="Aerospike" sheetId="4" r:id="rId5"/>
     <sheet name="Memcached" sheetId="5" r:id="rId6"/>
   </sheets>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="25">
   <si>
     <t>Redis</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Rea+Upd</t>
+  </si>
+  <si>
+    <t>Riak KV</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$16</c:f>
+              <c:f>'Workloads - Read, Update'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -244,14 +247,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read, Update'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -264,7 +267,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$22:$F$22</c:f>
+              <c:f>'Workloads - Read, Update'!$C$22:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -517,7 +520,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$16</c:f>
+              <c:f>'Workloads - Read, Update'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -538,14 +541,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read, Update'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -811,7 +814,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$17</c:f>
+              <c:f>'Workloads - Read, Update'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -832,14 +835,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read, Update'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -1105,7 +1108,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$5</c:f>
+              <c:f>'Workloads - Read, Update'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1126,14 +1129,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read, Update'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -1399,7 +1402,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$17</c:f>
+              <c:f>'Workloads - Read, Update'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1420,14 +1423,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read, Update'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -1440,7 +1443,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$23:$F$23</c:f>
+              <c:f>'Workloads - Read, Update'!$C$23:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1693,7 +1696,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$16</c:f>
+              <c:f>'Workloads - Read, Update'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1714,14 +1717,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Workloads - Read,Write'!$C$3:$E$3,'Workloads - Read,Write'!$F$3)</c:f>
+              <c:f>('Workloads - Read, Update'!$C$3:$E$3,'Workloads - Read, Update'!$F$3)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -1734,7 +1737,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$47:$F$47</c:f>
+              <c:f>'Workloads - Read, Update'!$C$47:$F$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1987,7 +1990,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$17</c:f>
+              <c:f>'Workloads - Read, Update'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2008,14 +2011,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Workloads - Read,Write'!$C$3:$E$3,'Workloads - Read,Write'!$F$3)</c:f>
+              <c:f>('Workloads - Read, Update'!$C$3:$E$3,'Workloads - Read, Update'!$F$3)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -2028,7 +2031,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$48:$F$48</c:f>
+              <c:f>'Workloads - Read, Update'!$C$48:$F$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2281,7 +2284,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$16</c:f>
+              <c:f>'Workloads - Read, Update'!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2302,14 +2305,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Workloads - Read,Write'!$C$3:$E$3,'Workloads - Read,Write'!$F$3)</c:f>
+              <c:f>('Workloads - Read, Update'!$C$3:$E$3,'Workloads - Read, Update'!$F$3)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -2322,7 +2325,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$60:$F$60</c:f>
+              <c:f>'Workloads - Read, Update'!$C$60:$F$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2575,7 +2578,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$17</c:f>
+              <c:f>'Workloads - Read, Update'!$B$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2596,14 +2599,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read, Update'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -2616,7 +2619,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$61:$F$61</c:f>
+              <c:f>'Workloads - Read, Update'!$C$61:$F$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2869,7 +2872,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$5</c:f>
+              <c:f>'Workloads - Read, Update'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2890,14 +2893,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read, Update'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -2910,7 +2913,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$5:$F$5</c:f>
+              <c:f>'Workloads - Read, Update'!$C$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3163,7 +3166,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$5</c:f>
+              <c:f>'Workloads - Read, Update'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3184,14 +3187,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Workloads - Read,Write'!$C$3:$E$3,'Workloads - Read,Write'!$F$3)</c:f>
+              <c:f>('Workloads - Read, Update'!$C$3:$E$3,'Workloads - Read, Update'!$F$3)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -3204,7 +3207,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$30:$F$30</c:f>
+              <c:f>'Workloads - Read, Update'!$C$30:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3457,7 +3460,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$B$5</c:f>
+              <c:f>'Workloads - Read, Update'!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3478,14 +3481,14 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Workloads - Read,Write'!$C$3:$F$3</c:f>
+              <c:f>'Workloads - Read, Update'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Redis</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Riak</c:v>
+                  <c:v>Riak KV</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Aerospike</c:v>
@@ -3498,7 +3501,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Workloads - Read,Write'!$C$55:$F$55</c:f>
+              <c:f>'Workloads - Read, Update'!$C$55:$F$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -10940,8 +10943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10963,7 +10966,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -10981,7 +10984,7 @@
         <v>208419</v>
       </c>
       <c r="D4">
-        <f>Riak!C8</f>
+        <f>'Riak KV'!C8</f>
         <v>803880.33333333337</v>
       </c>
       <c r="E4">
@@ -11002,7 +11005,7 @@
         <v>4801.03800056401</v>
       </c>
       <c r="D5">
-        <f>Riak!C9</f>
+        <f>'Riak KV'!C9</f>
         <v>1283.9777176479602</v>
       </c>
       <c r="E5">
@@ -11026,7 +11029,7 @@
         <v>500157</v>
       </c>
       <c r="D6">
-        <f>Riak!C10</f>
+        <f>'Riak KV'!C10</f>
         <v>500382</v>
       </c>
       <c r="E6">
@@ -11047,7 +11050,7 @@
         <v>836.76528222357695</v>
       </c>
       <c r="D7">
-        <f>Riak!C11</f>
+        <f>'Riak KV'!C11</f>
         <v>2175.8569730388999</v>
       </c>
       <c r="E7">
@@ -11068,7 +11071,7 @@
         <v>325.33333333333331</v>
       </c>
       <c r="D8">
-        <f>Riak!C12</f>
+        <f>'Riak KV'!C12</f>
         <v>861.33333333333337</v>
       </c>
       <c r="E8">
@@ -11089,7 +11092,7 @@
         <v>50473.666666666664</v>
       </c>
       <c r="D9">
-        <f>Riak!C13</f>
+        <f>'Riak KV'!C13</f>
         <v>158271</v>
       </c>
       <c r="E9">
@@ -11110,7 +11113,7 @@
         <v>1281.3333333333333</v>
       </c>
       <c r="D10">
-        <f>Riak!C14</f>
+        <f>'Riak KV'!C14</f>
         <v>3695</v>
       </c>
       <c r="E10">
@@ -11131,7 +11134,7 @@
         <v>1917.3333333333333</v>
       </c>
       <c r="D11">
-        <f>Riak!C15</f>
+        <f>'Riak KV'!C15</f>
         <v>7399</v>
       </c>
       <c r="E11">
@@ -11155,7 +11158,7 @@
         <v>499843</v>
       </c>
       <c r="D12">
-        <f>Riak!C16</f>
+        <f>'Riak KV'!C16</f>
         <v>499618</v>
       </c>
       <c r="E12">
@@ -11176,7 +11179,7 @@
         <v>824.12904984055911</v>
       </c>
       <c r="D13">
-        <f>Riak!C17</f>
+        <f>'Riak KV'!C17</f>
         <v>5941.3298998398968</v>
       </c>
       <c r="E13">
@@ -11197,7 +11200,7 @@
         <v>305</v>
       </c>
       <c r="D14">
-        <f>Riak!C18</f>
+        <f>'Riak KV'!C18</f>
         <v>2526.6666666666665</v>
       </c>
       <c r="E14">
@@ -11218,7 +11221,7 @@
         <v>45375</v>
       </c>
       <c r="D15">
-        <f>Riak!C19</f>
+        <f>'Riak KV'!C19</f>
         <v>167764.33333333334</v>
       </c>
       <c r="E15">
@@ -11239,7 +11242,7 @@
         <v>1264.6666666666667</v>
       </c>
       <c r="D16">
-        <f>Riak!C20</f>
+        <f>'Riak KV'!C20</f>
         <v>9819</v>
       </c>
       <c r="E16">
@@ -11260,7 +11263,7 @@
         <v>1891.6666666666667</v>
       </c>
       <c r="D17">
-        <f>Riak!C21</f>
+        <f>'Riak KV'!C21</f>
         <v>16332.333333333334</v>
       </c>
       <c r="E17">
@@ -11410,7 +11413,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E28" t="s">
         <v>2</v>
@@ -11428,7 +11431,7 @@
         <v>212026.33333333334</v>
       </c>
       <c r="D29">
-        <f>Riak!C27</f>
+        <f>'Riak KV'!C27</f>
         <v>562799.66666666663</v>
       </c>
       <c r="E29">
@@ -11449,7 +11452,7 @@
         <v>4726.9578685717897</v>
       </c>
       <c r="D30">
-        <f>Riak!C28</f>
+        <f>'Riak KV'!C28</f>
         <v>1778.1582630532967</v>
       </c>
       <c r="E30">
@@ -11473,7 +11476,7 @@
         <v>949836</v>
       </c>
       <c r="D31">
-        <f>Riak!C29</f>
+        <f>'Riak KV'!C29</f>
         <v>949728</v>
       </c>
       <c r="E31">
@@ -11494,7 +11497,7 @@
         <v>845.21823030995529</v>
       </c>
       <c r="D32">
-        <f>Riak!C30</f>
+        <f>'Riak KV'!C30</f>
         <v>2072.9082253935767</v>
       </c>
       <c r="E32">
@@ -11515,7 +11518,7 @@
         <v>313.66666666666669</v>
       </c>
       <c r="D33">
-        <f>Riak!C31</f>
+        <f>'Riak KV'!C31</f>
         <v>825.33333333333337</v>
       </c>
       <c r="E33">
@@ -11536,7 +11539,7 @@
         <v>50559</v>
       </c>
       <c r="D34">
-        <f>Riak!C32</f>
+        <f>'Riak KV'!C32</f>
         <v>110356.33333333333</v>
       </c>
       <c r="E34">
@@ -11557,7 +11560,7 @@
         <v>1325</v>
       </c>
       <c r="D35">
-        <f>Riak!C33</f>
+        <f>'Riak KV'!C33</f>
         <v>3232.3333333333335</v>
       </c>
       <c r="E35">
@@ -11578,7 +11581,7 @@
         <v>2232.3333333333335</v>
       </c>
       <c r="D36">
-        <f>Riak!C34</f>
+        <f>'Riak KV'!C34</f>
         <v>6805.666666666667</v>
       </c>
       <c r="E36">
@@ -11602,7 +11605,7 @@
         <v>50164</v>
       </c>
       <c r="D37">
-        <f>Riak!C35</f>
+        <f>'Riak KV'!C35</f>
         <v>50272</v>
       </c>
       <c r="E37">
@@ -11623,7 +11626,7 @@
         <v>841.38027581715448</v>
       </c>
       <c r="D38">
-        <f>Riak!C36</f>
+        <f>'Riak KV'!C36</f>
         <v>5827.5136784126071</v>
       </c>
       <c r="E38">
@@ -11644,7 +11647,7 @@
         <v>342</v>
       </c>
       <c r="D39">
-        <f>Riak!C37</f>
+        <f>'Riak KV'!C37</f>
         <v>2765.3333333333335</v>
       </c>
       <c r="E39">
@@ -11665,7 +11668,7 @@
         <v>41449.666666666664</v>
       </c>
       <c r="D40">
-        <f>Riak!C38</f>
+        <f>'Riak KV'!C38</f>
         <v>127231</v>
       </c>
       <c r="E40">
@@ -11686,7 +11689,7 @@
         <v>1322.3333333333333</v>
       </c>
       <c r="D41">
-        <f>Riak!C39</f>
+        <f>'Riak KV'!C39</f>
         <v>8903</v>
       </c>
       <c r="E41">
@@ -11707,7 +11710,7 @@
         <v>2243.3333333333335</v>
       </c>
       <c r="D42">
-        <f>Riak!C40</f>
+        <f>'Riak KV'!C40</f>
         <v>14495</v>
       </c>
       <c r="E42">
@@ -11857,7 +11860,7 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E53" t="s">
         <v>2</v>
@@ -11875,7 +11878,7 @@
         <v>205492.66666666666</v>
       </c>
       <c r="D54">
-        <f>Riak!C46</f>
+        <f>'Riak KV'!C46</f>
         <v>562029.33333333337</v>
       </c>
       <c r="E54">
@@ -11896,7 +11899,7 @@
         <v>4868.3014319549338</v>
       </c>
       <c r="D55">
-        <f>Riak!C47</f>
+        <f>'Riak KV'!C47</f>
         <v>1783.3907950035066</v>
       </c>
       <c r="E55">
@@ -11920,7 +11923,7 @@
         <v>1000000</v>
       </c>
       <c r="D56">
-        <f>Riak!C48</f>
+        <f>'Riak KV'!C48</f>
         <v>1000000</v>
       </c>
       <c r="E56">
@@ -11941,7 +11944,7 @@
         <v>819.3226933333334</v>
       </c>
       <c r="D57">
-        <f>Riak!C49</f>
+        <f>'Riak KV'!C49</f>
         <v>2241.0063320000004</v>
       </c>
       <c r="E57">
@@ -11962,7 +11965,7 @@
         <v>308.66666666666669</v>
       </c>
       <c r="D58">
-        <f>Riak!C50</f>
+        <f>'Riak KV'!C50</f>
         <v>804.66666666666663</v>
       </c>
       <c r="E58">
@@ -11983,7 +11986,7 @@
         <v>33935</v>
       </c>
       <c r="D59">
-        <f>Riak!C51</f>
+        <f>'Riak KV'!C51</f>
         <v>83903</v>
       </c>
       <c r="E59">
@@ -12004,7 +12007,7 @@
         <v>1213.3333333333333</v>
       </c>
       <c r="D60">
-        <f>Riak!C52</f>
+        <f>'Riak KV'!C52</f>
         <v>3714.3333333333335</v>
       </c>
       <c r="E60">
@@ -12025,7 +12028,7 @@
         <v>1856</v>
       </c>
       <c r="D61">
-        <f>Riak!C53</f>
+        <f>'Riak KV'!C53</f>
         <v>7885.666666666667</v>
       </c>
       <c r="E61">
@@ -12047,8 +12050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E628E191-458C-48C1-BA88-DA60FE101777}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12073,7 +12076,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -12234,7 +12237,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
@@ -12395,7 +12398,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E29" t="s">
         <v>2</v>
@@ -12556,7 +12559,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E42" t="s">
         <v>2</v>
@@ -13500,8 +13503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8B41AC-D64A-4E90-ABED-E837F425F881}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13512,7 +13515,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>